<commit_message>
Updated with Front-End Design
</commit_message>
<xml_diff>
--- a/Databases/Database.xlsx
+++ b/Databases/Database.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -711,7 +711,7 @@
         <v>28</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>1500.0</v>
+        <v>1000.0</v>
       </c>
       <c r="H5" t="n" s="0">
         <v>2200.0</v>

</xml_diff>